<commit_message>
feat: Introduce ADSP validation summary reporting with supporting sample data generation and header extraction logic.
</commit_message>
<xml_diff>
--- a/tests/sample_intake.xlsx
+++ b/tests/sample_intake.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,51 +429,31 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Section</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Field</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
+          <t>Fixing of FMS2134 job failure</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>HEADER</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Practice/Account</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Digital Transformation / AI Lab</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HEADER</t>
+          <t>Section</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Project Name</t>
+          <t>Field</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Intake Validator Pilot</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
@@ -485,12 +465,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ticket Hyperlink</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>BP-00479</t>
+          <t>Practice/Account</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Digital Transformation / AI Lab</t>
         </is>
       </c>
     </row>
@@ -502,14 +482,10 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2026-01-31</t>
-        </is>
-      </c>
+          <t>Project Name</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -519,46 +495,46 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Deadline</t>
+          <t>Ticket Hyperlink</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2026-03-15</t>
+          <t>BP-00479</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BUSINESS_CASE</t>
+          <t>HEADER</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Why now</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>The current manual process is slow and error-prone.</t>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>15-Jul-25</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BUSINESS_CASE</t>
+          <t>HEADER</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Consequences of delay</t>
+          <t>Deadline</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Increased turnaround time and potential data entry errors.</t>
+          <t>30-Sep-25</t>
         </is>
       </c>
     </row>
@@ -570,12 +546,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Technical justification</t>
+          <t>Why now</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Leveraging LLMs for semantic validation of unstructured text.</t>
+          <t>The current manual process is slow and error-prone.</t>
         </is>
       </c>
     </row>
@@ -587,12 +563,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Softtek Big Y</t>
+          <t>Consequences of delay</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Reduction in operational overhead.</t>
+          <t>Increased turnaround time and potential data entry errors.</t>
         </is>
       </c>
     </row>
@@ -604,46 +580,46 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Organizational KPI</t>
+          <t>Technical justification</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Efficiency improvement by 40%</t>
+          <t>Leveraging LLMs for semantic validation of unstructured text.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PROBLEM_STATEMENT</t>
+          <t>BUSINESS_CASE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Problem Definition</t>
+          <t>Softtek Big Y</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Project intake documents are often incomplete or inconsistent.</t>
+          <t>Reduction in operational overhead.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PROBLEM_STATEMENT</t>
+          <t>BUSINESS_CASE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Current Pain Points</t>
+          <t>Organizational KPI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Reviewers spend hours manually checking for mandatory information.</t>
+          <t>Efficiency improvement by 40%</t>
         </is>
       </c>
     </row>
@@ -655,12 +631,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Business/System Impact</t>
+          <t>Problem Definition</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Delays in project kickoff and resource allocation.</t>
+          <t>Project intake documents are often incomplete or inconsistent.</t>
         </is>
       </c>
     </row>
@@ -672,80 +648,80 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Who is affected</t>
+          <t>Current Pain Points</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Project Management Office (PMO) and Delivery Teams.</t>
+          <t>Reviewers spend hours manually checking for mandatory information.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PROJECT_SCOPE</t>
+          <t>PROBLEM_STATEMENT</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>In Scope</t>
+          <t>Business/System Impact</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Azure OpenAI integration, PDF/Excel support, LangGraph orchestration.</t>
+          <t>Delays in project kickoff and resource allocation.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PROJECT_SCOPE</t>
+          <t>PROBLEM_STATEMENT</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Out of Scope</t>
+          <t>Who is affected</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Legacy system migration, SAP integration.</t>
+          <t>Project Management Office (PMO) and Delivery Teams.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EXPECTED_BENEFITS</t>
+          <t>PROJECT_SCOPE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Qualitative Benefits</t>
+          <t>In Scope</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Improved data quality and faster approval cycles.</t>
+          <t>Azure OpenAI integration, PDF/Excel support, LangGraph orchestration.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EXPECTED_BENEFITS</t>
+          <t>PROJECT_SCOPE</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Softtek Hard Dollars</t>
+          <t>Out of Scope</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$50,000</t>
+          <t>Legacy system migration, SAP integration.</t>
         </is>
       </c>
     </row>
@@ -757,12 +733,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Softtek Soft Dollars</t>
+          <t>Qualitative Benefits</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$10,000</t>
+          <t>Improved data quality and faster approval cycles.</t>
         </is>
       </c>
     </row>
@@ -774,12 +750,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Customer Hard Dollars</t>
+          <t>Softtek Hard Dollars</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$100,000</t>
+          <t>$50,000</t>
         </is>
       </c>
     </row>
@@ -791,10 +767,44 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Softtek Soft Dollars</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$10,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>EXPECTED_BENEFITS</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Customer Hard Dollars</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$100,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>EXPECTED_BENEFITS</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>Customer Soft Dollars</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>$20,000</t>
         </is>
@@ -802,7 +812,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>